<commit_message>
Added architectural design review
</commit_message>
<xml_diff>
--- a/Docs/initial/Lab01_ReviewReport.xlsx
+++ b/Docs/initial/Lab01_ReviewReport.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facultate\Semestrul 6\VVSS\Raspy-Tasks\Docs\initial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Faculta\vvss\Raspy-Tasks\Docs\initial\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86236DE3-74E2-4FA4-B896-FA739C2DC000}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="150" windowWidth="14160" windowHeight="8265" tabRatio="650"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="650" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -17,12 +18,20 @@
     <sheet name="Coding Phase Defects" sheetId="5" r:id="rId3"/>
     <sheet name="DynamicCodeAnalysis" sheetId="8" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="65">
   <si>
     <t>Document  Title:</t>
   </si>
@@ -172,19 +181,71 @@
   </si>
   <si>
     <t>Detaliile unui task nu includ starea de activ sau inactiv - nu se precizeaza cum este stocata starea unui task</t>
+  </si>
+  <si>
+    <t>Gaidur Ioan</t>
+  </si>
+  <si>
+    <t>Gaspar Patricia Lorena</t>
+  </si>
+  <si>
+    <t>Gheorghiu Dragos</t>
+  </si>
+  <si>
+    <t>Gheorghiu Dragos Constantin</t>
+  </si>
+  <si>
+    <t>18.03.2020</t>
+  </si>
+  <si>
+    <t>A01</t>
+  </si>
+  <si>
+    <t>A02</t>
+  </si>
+  <si>
+    <t>A03</t>
+  </si>
+  <si>
+    <t>A05</t>
+  </si>
+  <si>
+    <t>NewEditController</t>
+  </si>
+  <si>
+    <t>New and Edit windows should have separate controllers, that means separate files too</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>yes, it accounts for the requirements</t>
+  </si>
+  <si>
+    <t>There is no master exception handling</t>
+  </si>
+  <si>
+    <t>it is logically and correctly partitioned</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -356,82 +417,84 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,6 +588,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -560,6 +640,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -735,14 +832,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F5" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,8 +848,9 @@
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
     <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="21" style="6" customWidth="1"/>
+    <col min="6" max="7" width="8.85546875" style="6"/>
+    <col min="8" max="8" width="12.140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="34.140625" style="6" customWidth="1"/>
     <col min="10" max="10" width="14.42578125" style="6" customWidth="1"/>
     <col min="11" max="16384" width="8.85546875" style="6"/>
   </cols>
@@ -762,19 +860,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>31</v>
@@ -784,54 +882,66 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="I3" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="18">
+        <v>233</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="24"/>
+      <c r="E4" s="26"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="3">
+        <v>233</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="26"/>
+      <c r="E5" s="28"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="3">
+        <v>233</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -846,7 +956,7 @@
       <c r="E9" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="G9" s="36"/>
+      <c r="G9" s="22"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
@@ -859,10 +969,10 @@
         <v>1</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="35" t="s">
+      <c r="F10" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="21" t="s">
         <v>47</v>
       </c>
     </row>
@@ -878,10 +988,10 @@
         <v>1</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="35" t="s">
+      <c r="F11" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G11" s="35" t="s">
+      <c r="G11" s="21" t="s">
         <v>49</v>
       </c>
     </row>
@@ -893,10 +1003,10 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="35" t="s">
+      <c r="F12" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="35" t="s">
+      <c r="G12" s="21" t="s">
         <v>39</v>
       </c>
     </row>
@@ -908,10 +1018,10 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="35" t="s">
+      <c r="F13" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G13" s="35" t="s">
+      <c r="G13" s="21" t="s">
         <v>46</v>
       </c>
     </row>
@@ -923,10 +1033,10 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="35" t="s">
+      <c r="F14" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="G14" s="35" t="s">
+      <c r="G14" s="21" t="s">
         <v>40</v>
       </c>
     </row>
@@ -938,7 +1048,7 @@
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="35" t="s">
+      <c r="F15" s="21" t="s">
         <v>35</v>
       </c>
       <c r="G15" s="6" t="s">
@@ -953,10 +1063,10 @@
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="35" t="s">
+      <c r="F16" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="35" t="s">
+      <c r="G16" s="21" t="s">
         <v>48</v>
       </c>
     </row>
@@ -968,10 +1078,10 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="35" t="s">
+      <c r="F17" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="35" t="s">
+      <c r="G17" s="21" t="s">
         <v>41</v>
       </c>
     </row>
@@ -983,10 +1093,10 @@
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="16"/>
-      <c r="F18" s="35" t="s">
+      <c r="F18" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="35" t="s">
+      <c r="G18" s="21" t="s">
         <v>42</v>
       </c>
     </row>
@@ -998,7 +1108,7 @@
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
       <c r="E19" s="16"/>
-      <c r="G19" s="35" t="s">
+      <c r="G19" s="21" t="s">
         <v>43</v>
       </c>
     </row>
@@ -1010,7 +1120,7 @@
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
       <c r="E20" s="16"/>
-      <c r="G20" s="35" t="s">
+      <c r="G20" s="21" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1022,7 +1132,7 @@
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
       <c r="E21" s="16"/>
-      <c r="G21" s="35" t="s">
+      <c r="G21" s="21" t="s">
         <v>45</v>
       </c>
     </row>
@@ -1087,24 +1197,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" style="6"/>
     <col min="2" max="2" width="12.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="16.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
-    <col min="9" max="9" width="22" style="6" customWidth="1"/>
+    <col min="6" max="7" width="8.85546875" style="6"/>
+    <col min="8" max="8" width="10.28515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="29.85546875" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
@@ -1113,19 +1225,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>31</v>
@@ -1135,54 +1247,70 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="I3" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="18">
+        <v>233</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="27"/>
+      <c r="E4" s="29"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="3">
+        <v>233</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="28" t="s">
+      <c r="D5" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="29"/>
+      <c r="E5" s="31"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="3">
+        <v>233</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1198,40 +1326,64 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="C10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
         <f>B10+1</f>
         <v>2</v>
       </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="C11" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" s="3">
         <f t="shared" ref="B12:B26" si="0">B11+1</f>
         <v>3</v>
       </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="2"/>
+      <c r="C12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B13" s="3">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
+      <c r="C13" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="3">
@@ -1358,7 +1510,9 @@
         <v>8</v>
       </c>
       <c r="D28" s="13"/>
-      <c r="E28" s="1"/>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -1375,14 +1529,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,7 +1546,8 @@
     <col min="3" max="3" width="16.28515625" style="6" customWidth="1"/>
     <col min="4" max="4" width="18" style="6" customWidth="1"/>
     <col min="5" max="5" width="41.42578125" style="6" customWidth="1"/>
-    <col min="6" max="8" width="8.85546875" style="6"/>
+    <col min="6" max="7" width="8.85546875" style="6"/>
+    <col min="8" max="8" width="12.140625" style="6" customWidth="1"/>
     <col min="9" max="9" width="26.7109375" style="6" customWidth="1"/>
     <col min="10" max="16384" width="8.85546875" style="6"/>
   </cols>
@@ -1402,19 +1557,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>31</v>
@@ -1427,51 +1582,63 @@
       <c r="H3" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
+      <c r="I3" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="18">
+        <v>233</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="30" t="s">
+      <c r="D4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="30"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="I4" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="3">
+        <v>233</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="32"/>
+      <c r="E5" s="34"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="I5" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="J5" s="3">
+        <v>233</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="C7" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -1491,9 +1658,6 @@
       <c r="B10" s="3">
         <v>1</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B11" s="3">
@@ -1700,7 +1864,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="6" tint="0.79998168889431442"/>
   </sheetPr>
@@ -1728,19 +1892,19 @@
       <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="H1" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
       <c r="H2" s="3"/>
       <c r="I2" s="20" t="s">
         <v>31</v>
@@ -1760,8 +1924,8 @@
       <c r="C4" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
       <c r="H4" s="18" t="s">
         <v>21</v>
       </c>
@@ -1772,8 +1936,8 @@
       <c r="C5" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
       </c>
@@ -1785,8 +1949,8 @@
       <c r="C6" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
@@ -2018,11 +2182,11 @@
       <c r="E31" s="11"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C32" s="33" t="s">
+      <c r="C32" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="D32" s="34"/>
-      <c r="E32" s="34"/>
+      <c r="D32" s="36"/>
+      <c r="E32" s="36"/>
       <c r="F32" s="19"/>
     </row>
   </sheetData>

</xml_diff>